<commit_message>
newest version of assignment 3
</commit_message>
<xml_diff>
--- a/Intro to Machine Learning/Assignment_3_ Submission_Template.xlsx
+++ b/Intro to Machine Learning/Assignment_3_ Submission_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shashi\Downloads\Contracts\UCSC\UCSC Ext\Resources_09_2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lye\Documents\GitHub\python-assignments\Intro to Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19872" windowHeight="8436" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -3901,7 +3901,7 @@
     <t>[Optional] Type your observations on PCA, histogram classifiers and Bayesian classifiers in this space.</t>
   </si>
   <si>
-    <t>STUDENT NAME (REQUIRED)</t>
+    <t>Laura Ye</t>
   </si>
 </sst>
 </file>
@@ -4365,8 +4365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ADE98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35943,7 +35943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>